<commit_message>
Change 'sample data' file name to 'sample_name'
</commit_message>
<xml_diff>
--- a/sample_data/radar_colours.xlsx
+++ b/sample_data/radar_colours.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cxwhite\Pycharm\playground\sample data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswhite/PycharmProjects/radar_prediction/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>B</t>
   </si>
@@ -36,12 +36,6 @@
   </si>
   <si>
     <t>mm/hr</t>
-  </si>
-  <si>
-    <t>Not visible</t>
-  </si>
-  <si>
-    <t>Off-white</t>
   </si>
   <si>
     <t>Sky-blue</t>
@@ -95,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,18 +105,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -236,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -281,9 +269,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -566,21 +551,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -595,395 +580,353 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="16">
+        <v>255</v>
+      </c>
+      <c r="E2" s="16">
+        <v>180</v>
+      </c>
+      <c r="F2" s="16">
+        <v>180</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="16">
         <v>255</v>
       </c>
-      <c r="E3" s="17">
-        <v>245</v>
-      </c>
-      <c r="F3" s="17">
-        <v>245</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="16">
+        <v>120</v>
+      </c>
+      <c r="F3" s="16">
+        <v>120</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="17">
+        <v>4</v>
+      </c>
+      <c r="D4" s="16">
         <v>255</v>
       </c>
-      <c r="E4" s="17">
-        <v>180</v>
-      </c>
-      <c r="F4" s="17">
-        <v>180</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="16">
+        <v>20</v>
+      </c>
+      <c r="F4" s="16">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D5" s="17">
-        <v>255</v>
-      </c>
-      <c r="E5" s="17">
-        <v>120</v>
-      </c>
-      <c r="F5" s="17">
-        <v>120</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D5" s="16">
+        <v>195</v>
+      </c>
+      <c r="E5" s="16">
+        <v>216</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="17">
-        <v>255</v>
-      </c>
-      <c r="E6" s="17">
-        <v>20</v>
-      </c>
-      <c r="F6" s="17">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D6" s="16">
+        <v>144</v>
+      </c>
+      <c r="E6" s="16">
+        <v>150</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7" s="17">
-        <v>195</v>
-      </c>
-      <c r="E7" s="17">
-        <v>216</v>
-      </c>
-      <c r="F7" s="17">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D7" s="16">
+        <v>102</v>
+      </c>
+      <c r="E7" s="16">
+        <v>102</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>10</v>
-      </c>
-      <c r="D8" s="17">
-        <v>144</v>
-      </c>
-      <c r="E8" s="17">
-        <v>150</v>
-      </c>
-      <c r="F8" s="17">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <v>255</v>
+      </c>
+      <c r="F8" s="16">
+        <v>255</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>15</v>
-      </c>
-      <c r="D9" s="17">
-        <v>102</v>
-      </c>
-      <c r="E9" s="17">
-        <v>102</v>
-      </c>
-      <c r="F9" s="17">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>200</v>
+      </c>
+      <c r="F9" s="16">
+        <v>255</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>20</v>
-      </c>
-      <c r="D10" s="17">
-        <v>0</v>
-      </c>
-      <c r="E10" s="17">
+        <v>50</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>150</v>
+      </c>
+      <c r="F10" s="16">
         <v>255</v>
       </c>
-      <c r="F10" s="17">
-        <v>255</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>35</v>
-      </c>
-      <c r="D11" s="17">
-        <v>0</v>
-      </c>
-      <c r="E11" s="17">
-        <v>200</v>
-      </c>
-      <c r="F11" s="17">
+        <v>80</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>100</v>
+      </c>
+      <c r="F11" s="16">
         <v>255</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="11"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1">
-        <v>50</v>
-      </c>
-      <c r="D12" s="17">
-        <v>0</v>
-      </c>
-      <c r="E12" s="17">
-        <v>150</v>
-      </c>
-      <c r="F12" s="17">
+        <v>120</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
         <v>255</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="G12" s="12"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>80</v>
-      </c>
-      <c r="D13" s="17">
-        <v>0</v>
-      </c>
-      <c r="E13" s="17">
-        <v>100</v>
-      </c>
-      <c r="F13" s="17">
-        <v>255</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>200</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1">
+        <v>300</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
         <v>120</v>
       </c>
-      <c r="D14" s="17">
-        <v>0</v>
-      </c>
-      <c r="E14" s="17">
-        <v>0</v>
-      </c>
-      <c r="F14" s="17">
-        <v>255</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="14"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="1">
-        <v>200</v>
-      </c>
-      <c r="D15" s="17">
-        <v>0</v>
-      </c>
-      <c r="E15" s="17">
-        <v>0</v>
-      </c>
-      <c r="F15" s="17">
-        <v>200</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1">
-        <v>300</v>
-      </c>
-      <c r="D16" s="17">
-        <v>0</v>
-      </c>
-      <c r="E16" s="17">
-        <v>0</v>
-      </c>
-      <c r="F16" s="17">
-        <v>120</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1">
         <v>360</v>
       </c>
-      <c r="D17" s="17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
         <v>40</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>